<commit_message>
bissl zeug gmacht lul
</commit_message>
<xml_diff>
--- a/__ideen_zu_fourfoil/reserved_words.xlsx
+++ b/__ideen_zu_fourfoil/reserved_words.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t xml:space="preserve">defs</t>
   </si>
@@ -61,25 +61,16 @@
     <t xml:space="preserve">private</t>
   </si>
   <si>
-    <t xml:space="preserve">'' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'a' is a char</t>
-  </si>
-  <si>
     <t xml:space="preserve">print( String x )</t>
   </si>
   <si>
     <t xml:space="preserve">fun</t>
   </si>
   <si>
-    <t xml:space="preserve">char</t>
-  </si>
-  <si>
     <t xml:space="preserve"># </t>
   </si>
   <si>
-    <t xml:space="preserve">#234 is an int</t>
+    <t xml:space="preserve">#234 is an int in hex format</t>
   </si>
   <si>
     <t xml:space="preserve">println( String x )</t>
@@ -88,9 +79,6 @@
     <t xml:space="preserve">ptr</t>
   </si>
   <si>
-    <t xml:space="preserve">short</t>
-  </si>
-  <si>
     <t xml:space="preserve">=</t>
   </si>
   <si>
@@ -115,16 +103,13 @@
     <t xml:space="preserve">addition</t>
   </si>
   <si>
-    <t xml:space="preserve">long</t>
-  </si>
-  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">subtraction</t>
   </si>
   <si>
-    <t xml:space="preserve">free</t>
+    <t xml:space="preserve">del</t>
   </si>
   <si>
     <t xml:space="preserve">float</t>
@@ -142,9 +127,6 @@
     <t xml:space="preserve">return</t>
   </si>
   <si>
-    <t xml:space="preserve">double</t>
-  </si>
-  <si>
     <t xml:space="preserve">/</t>
   </si>
   <si>
@@ -157,6 +139,12 @@
     <t xml:space="preserve">switch</t>
   </si>
   <si>
+    <t xml:space="preserve">'a’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a is a non-unicode string</t>
+  </si>
+  <si>
     <t xml:space="preserve">case</t>
   </si>
   <si>
@@ -217,13 +205,10 @@
     <t xml:space="preserve">catch</t>
   </si>
   <si>
-    <t xml:space="preserve">||</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreach</t>
+    <t xml:space="preserve">|a|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount of a</t>
   </si>
 </sst>
 </file>
@@ -348,14 +333,16 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="22.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="22.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,7 +380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -403,214 +390,199 @@
       <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>